<commit_message>
add free upgrade options
</commit_message>
<xml_diff>
--- a/src/mesbg_options.xlsx
+++ b/src/mesbg_options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9CFACF-6F56-4AC2-A51B-1BD7DCB87696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF178789-835C-40C0-A828-0EE78D0A6AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2C0E6438-1EB7-4493-91C9-83873EACB085}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1120" uniqueCount="469">
   <si>
     <t>faction</t>
   </si>
@@ -1422,6 +1422,27 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>Anduril Flame of the West - FREE</t>
+  </si>
+  <si>
+    <t>Black Dragon Upgrade - FREE</t>
+  </si>
+  <si>
+    <t>Marauder Upgrade - FREE</t>
+  </si>
+  <si>
+    <t>OPT0275</t>
+  </si>
+  <si>
+    <t>OPT0276</t>
+  </si>
+  <si>
+    <t>OPT0277</t>
+  </si>
+  <si>
+    <t>OPT0278</t>
   </si>
 </sst>
 </file>
@@ -1816,10 +1837,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{301D72E7-4EC7-4027-A18B-32FBE399A765}">
-  <dimension ref="A1:H275"/>
+  <dimension ref="A1:H279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="H88" sqref="H88"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2516,13 +2537,13 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>463</v>
       </c>
       <c r="E27">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F27" t="b">
         <v>0</v>
@@ -2542,13 +2563,13 @@
         <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E28">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
@@ -2571,10 +2592,10 @@
         <v>34</v>
       </c>
       <c r="D29" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F29" t="b">
         <v>0</v>
@@ -2597,7 +2618,7 @@
         <v>34</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -2623,13 +2644,13 @@
         <v>34</v>
       </c>
       <c r="D31" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="F31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -2649,13 +2670,13 @@
         <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -2669,16 +2690,16 @@
         <v>216</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E33">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="F33" t="b">
         <v>0</v>
@@ -2695,16 +2716,16 @@
         <v>217</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
+        <v>463</v>
       </c>
       <c r="E34">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F34" t="b">
         <v>0</v>
@@ -2727,10 +2748,10 @@
         <v>37</v>
       </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E35">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="F35" t="b">
         <v>0</v>
@@ -2753,10 +2774,10 @@
         <v>37</v>
       </c>
       <c r="D36" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F36" t="b">
         <v>0</v>
@@ -2776,13 +2797,13 @@
         <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
         <v>25</v>
       </c>
       <c r="E37">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F37" t="b">
         <v>0</v>
@@ -2802,13 +2823,13 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D38" t="s">
         <v>38</v>
       </c>
       <c r="E38">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F38" t="b">
         <v>0</v>
@@ -2825,16 +2846,16 @@
         <v>222</v>
       </c>
       <c r="B39" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="E39">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
@@ -2851,16 +2872,16 @@
         <v>223</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F40" t="b">
         <v>0</v>
@@ -2880,13 +2901,13 @@
         <v>40</v>
       </c>
       <c r="C41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D41" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E41">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F41" t="b">
         <v>0</v>
@@ -2906,10 +2927,10 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -2932,13 +2953,13 @@
         <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E43">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F43" t="b">
         <v>0</v>
@@ -2958,13 +2979,13 @@
         <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="E44">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F44" t="b">
         <v>0</v>
@@ -2984,13 +3005,13 @@
         <v>40</v>
       </c>
       <c r="C45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="E45">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F45" t="b">
         <v>0</v>
@@ -3010,13 +3031,13 @@
         <v>40</v>
       </c>
       <c r="C46" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D46" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E46">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F46" t="b">
         <v>0</v>
@@ -3036,7 +3057,7 @@
         <v>40</v>
       </c>
       <c r="C47" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
@@ -3065,7 +3086,7 @@
         <v>50</v>
       </c>
       <c r="D48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E48">
         <v>5</v>
@@ -3088,13 +3109,13 @@
         <v>40</v>
       </c>
       <c r="C49" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E49">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F49" t="b">
         <v>0</v>
@@ -3114,13 +3135,13 @@
         <v>40</v>
       </c>
       <c r="C50" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F50" t="b">
         <v>0</v>
@@ -3143,13 +3164,13 @@
         <v>53</v>
       </c>
       <c r="D51" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -3169,7 +3190,7 @@
         <v>53</v>
       </c>
       <c r="D52" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -3192,16 +3213,16 @@
         <v>40</v>
       </c>
       <c r="C53" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D53" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="E53">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -3218,16 +3239,16 @@
         <v>40</v>
       </c>
       <c r="C54" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D54" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -3244,13 +3265,13 @@
         <v>40</v>
       </c>
       <c r="C55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D55" t="s">
-        <v>35</v>
+        <v>464</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" t="b">
         <v>0</v>
@@ -3273,10 +3294,10 @@
         <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F56" t="b">
         <v>0</v>
@@ -3293,19 +3314,19 @@
         <v>240</v>
       </c>
       <c r="B57" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C57" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D57" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E57">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -3319,16 +3340,16 @@
         <v>241</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C58" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D58" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="E58">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F58" t="b">
         <v>0</v>
@@ -3345,16 +3366,16 @@
         <v>242</v>
       </c>
       <c r="B59" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C59" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
       </c>
       <c r="E59">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F59" t="b">
         <v>0</v>
@@ -3374,13 +3395,13 @@
         <v>57</v>
       </c>
       <c r="C60" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D60" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="E60">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F60" t="b">
         <v>0</v>
@@ -3400,10 +3421,10 @@
         <v>57</v>
       </c>
       <c r="C61" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D61" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E61">
         <v>5</v>
@@ -3426,7 +3447,7 @@
         <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D62" t="s">
         <v>7</v>
@@ -3452,13 +3473,13 @@
         <v>57</v>
       </c>
       <c r="C63" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D63" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E63">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F63" t="b">
         <v>0</v>
@@ -3478,16 +3499,16 @@
         <v>57</v>
       </c>
       <c r="C64" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D64" t="s">
         <v>62</v>
       </c>
       <c r="E64">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F64" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -3504,13 +3525,13 @@
         <v>57</v>
       </c>
       <c r="C65" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D65" t="s">
         <v>7</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F65" t="b">
         <v>0</v>
@@ -3530,13 +3551,13 @@
         <v>57</v>
       </c>
       <c r="C66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D66" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E66">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F66" t="b">
         <v>0</v>
@@ -3556,16 +3577,16 @@
         <v>57</v>
       </c>
       <c r="C67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D67" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="E67">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="F67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -3582,16 +3603,16 @@
         <v>57</v>
       </c>
       <c r="C68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D68" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="E68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F68" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -3611,10 +3632,10 @@
         <v>64</v>
       </c>
       <c r="D69" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F69" t="b">
         <v>0</v>
@@ -3637,10 +3658,10 @@
         <v>64</v>
       </c>
       <c r="D70" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F70" t="b">
         <v>0</v>
@@ -3660,16 +3681,16 @@
         <v>57</v>
       </c>
       <c r="C71" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D71" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E71">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="F71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -3686,13 +3707,13 @@
         <v>57</v>
       </c>
       <c r="C72" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D72" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="E72">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F72" t="b">
         <v>0</v>
@@ -3712,13 +3733,13 @@
         <v>57</v>
       </c>
       <c r="C73" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D73" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E73">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F73" t="b">
         <v>0</v>
@@ -3738,13 +3759,13 @@
         <v>57</v>
       </c>
       <c r="C74" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D74" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E74">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F74" t="b">
         <v>0</v>
@@ -3764,13 +3785,13 @@
         <v>57</v>
       </c>
       <c r="C75" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D75" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E75">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F75" t="b">
         <v>0</v>
@@ -3790,13 +3811,13 @@
         <v>57</v>
       </c>
       <c r="C76" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D76" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="E76">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F76" t="b">
         <v>0</v>
@@ -3816,7 +3837,7 @@
         <v>57</v>
       </c>
       <c r="C77" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D77" t="s">
         <v>62</v>
@@ -3842,10 +3863,10 @@
         <v>57</v>
       </c>
       <c r="C78" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D78" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E78">
         <v>5</v>
@@ -3868,10 +3889,10 @@
         <v>57</v>
       </c>
       <c r="C79" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D79" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E79">
         <v>5</v>
@@ -3894,13 +3915,13 @@
         <v>57</v>
       </c>
       <c r="C80" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D80" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="E80">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F80" t="b">
         <v>0</v>
@@ -3920,16 +3941,16 @@
         <v>57</v>
       </c>
       <c r="C81" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D81" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="E81">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F81" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -3946,13 +3967,13 @@
         <v>57</v>
       </c>
       <c r="C82" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D82" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E82">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F82" t="b">
         <v>0</v>
@@ -3975,10 +3996,10 @@
         <v>75</v>
       </c>
       <c r="D83" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F83" t="b">
         <v>0</v>
@@ -4001,13 +4022,13 @@
         <v>75</v>
       </c>
       <c r="D84" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E84">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F84" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -4021,16 +4042,16 @@
         <v>268</v>
       </c>
       <c r="B85" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="C85" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D85" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="E85">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F85" t="b">
         <v>0</v>
@@ -4047,16 +4068,16 @@
         <v>269</v>
       </c>
       <c r="B86" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="C86" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D86" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E86">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="F86" t="b">
         <v>0</v>
@@ -4073,16 +4094,16 @@
         <v>270</v>
       </c>
       <c r="B87" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="C87" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D87" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E87">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F87" t="b">
         <v>0</v>
@@ -4102,13 +4123,13 @@
         <v>77</v>
       </c>
       <c r="C88" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D88" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E88">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F88" t="b">
         <v>0</v>
@@ -4117,7 +4138,7 @@
         <v>0</v>
       </c>
       <c r="H88">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
@@ -4128,13 +4149,13 @@
         <v>77</v>
       </c>
       <c r="C89" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D89" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="E89">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="F89" t="b">
         <v>0</v>
@@ -4154,13 +4175,13 @@
         <v>77</v>
       </c>
       <c r="C90" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D90" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E90">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F90" t="b">
         <v>0</v>
@@ -4180,13 +4201,13 @@
         <v>77</v>
       </c>
       <c r="C91" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D91" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="E91">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F91" t="b">
         <v>0</v>
@@ -4195,7 +4216,7 @@
         <v>0</v>
       </c>
       <c r="H91">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
@@ -4206,10 +4227,10 @@
         <v>77</v>
       </c>
       <c r="C92" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D92" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E92">
         <v>5</v>
@@ -4235,10 +4256,10 @@
         <v>83</v>
       </c>
       <c r="D93" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="E93">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="F93" t="b">
         <v>0</v>
@@ -4258,7 +4279,7 @@
         <v>77</v>
       </c>
       <c r="C94" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D94" t="s">
         <v>42</v>
@@ -4284,10 +4305,10 @@
         <v>77</v>
       </c>
       <c r="C95" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D95" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E95">
         <v>5</v>
@@ -4310,10 +4331,10 @@
         <v>77</v>
       </c>
       <c r="C96" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D96" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="E96">
         <v>5</v>
@@ -4339,10 +4360,10 @@
         <v>85</v>
       </c>
       <c r="D97" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="E97">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F97" t="b">
         <v>0</v>
@@ -4362,13 +4383,13 @@
         <v>77</v>
       </c>
       <c r="C98" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D98" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E98">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F98" t="b">
         <v>0</v>
@@ -4388,16 +4409,16 @@
         <v>77</v>
       </c>
       <c r="C99" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D99" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F99" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -4414,13 +4435,13 @@
         <v>77</v>
       </c>
       <c r="C100" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D100" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E100">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F100" t="b">
         <v>0</v>
@@ -4440,13 +4461,13 @@
         <v>77</v>
       </c>
       <c r="C101" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D101" t="s">
         <v>42</v>
       </c>
       <c r="E101">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F101" t="b">
         <v>0</v>
@@ -4466,16 +4487,16 @@
         <v>77</v>
       </c>
       <c r="C102" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D102" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="E102">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F102" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -4495,10 +4516,10 @@
         <v>88</v>
       </c>
       <c r="D103" t="s">
-        <v>59</v>
+        <v>25</v>
       </c>
       <c r="E103">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F103" t="b">
         <v>0</v>
@@ -4521,10 +4542,10 @@
         <v>88</v>
       </c>
       <c r="D104" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E104">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F104" t="b">
         <v>0</v>
@@ -4547,7 +4568,7 @@
         <v>88</v>
       </c>
       <c r="D105" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="E105">
         <v>5</v>
@@ -4570,13 +4591,13 @@
         <v>77</v>
       </c>
       <c r="C106" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D106" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="E106">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F106" t="b">
         <v>0</v>
@@ -4596,13 +4617,13 @@
         <v>77</v>
       </c>
       <c r="C107" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D107" t="s">
-        <v>92</v>
+        <v>38</v>
       </c>
       <c r="E107">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F107" t="b">
         <v>0</v>
@@ -4622,13 +4643,13 @@
         <v>77</v>
       </c>
       <c r="C108" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D108" t="s">
         <v>7</v>
       </c>
       <c r="E108">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F108" t="b">
         <v>0</v>
@@ -4648,13 +4669,13 @@
         <v>77</v>
       </c>
       <c r="C109" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D109" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="E109">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F109" t="b">
         <v>0</v>
@@ -4674,10 +4695,10 @@
         <v>77</v>
       </c>
       <c r="C110" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D110" t="s">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="E110">
         <v>25</v>
@@ -4700,7 +4721,7 @@
         <v>77</v>
       </c>
       <c r="C111" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D111" t="s">
         <v>7</v>
@@ -4726,16 +4747,16 @@
         <v>77</v>
       </c>
       <c r="C112" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D112" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="E112">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F112" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -4752,13 +4773,13 @@
         <v>77</v>
       </c>
       <c r="C113" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D113" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E113">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F113" t="b">
         <v>0</v>
@@ -4778,10 +4799,10 @@
         <v>77</v>
       </c>
       <c r="C114" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D114" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E114">
         <v>1</v>
@@ -4804,16 +4825,16 @@
         <v>77</v>
       </c>
       <c r="C115" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D115" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="E115">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F115" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -4830,10 +4851,10 @@
         <v>77</v>
       </c>
       <c r="C116" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D116" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E116">
         <v>1</v>
@@ -4856,13 +4877,13 @@
         <v>77</v>
       </c>
       <c r="C117" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D117" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E117">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F117" t="b">
         <v>0</v>
@@ -4882,13 +4903,13 @@
         <v>77</v>
       </c>
       <c r="C118" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D118" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="E118">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F118" t="b">
         <v>0</v>
@@ -4908,16 +4929,16 @@
         <v>77</v>
       </c>
       <c r="C119" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D119" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E119">
         <v>1</v>
       </c>
       <c r="F119" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -4937,10 +4958,10 @@
         <v>98</v>
       </c>
       <c r="D120" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E120">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F120" t="b">
         <v>0</v>
@@ -4963,10 +4984,10 @@
         <v>98</v>
       </c>
       <c r="D121" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E121">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F121" t="b">
         <v>0</v>
@@ -4983,19 +5004,19 @@
         <v>305</v>
       </c>
       <c r="B122" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="C122" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D122" t="s">
-        <v>101</v>
+        <v>28</v>
       </c>
       <c r="E122">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F122" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -5009,16 +5030,16 @@
         <v>306</v>
       </c>
       <c r="B123" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="C123" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D123" t="s">
-        <v>102</v>
+        <v>7</v>
       </c>
       <c r="E123">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F123" t="b">
         <v>0</v>
@@ -5035,16 +5056,16 @@
         <v>307</v>
       </c>
       <c r="B124" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="C124" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D124" t="s">
-        <v>103</v>
+        <v>8</v>
       </c>
       <c r="E124">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F124" t="b">
         <v>0</v>
@@ -5067,10 +5088,10 @@
         <v>100</v>
       </c>
       <c r="D125" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="E125">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F125" t="b">
         <v>0</v>
@@ -5093,10 +5114,10 @@
         <v>100</v>
       </c>
       <c r="D126" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="E126">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F126" t="b">
         <v>0</v>
@@ -5119,10 +5140,10 @@
         <v>100</v>
       </c>
       <c r="D127" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="E127">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F127" t="b">
         <v>0</v>
@@ -5139,16 +5160,16 @@
         <v>311</v>
       </c>
       <c r="B128" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C128" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D128" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="E128">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F128" t="b">
         <v>0</v>
@@ -5165,13 +5186,13 @@
         <v>312</v>
       </c>
       <c r="B129" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C129" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D129" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E129">
         <v>10</v>
@@ -5191,13 +5212,13 @@
         <v>313</v>
       </c>
       <c r="B130" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C130" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D130" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="E130">
         <v>5</v>
@@ -5220,13 +5241,13 @@
         <v>104</v>
       </c>
       <c r="C131" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D131" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="E131">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F131" t="b">
         <v>0</v>
@@ -5246,13 +5267,13 @@
         <v>104</v>
       </c>
       <c r="C132" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D132" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E132">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F132" t="b">
         <v>0</v>
@@ -5272,13 +5293,13 @@
         <v>104</v>
       </c>
       <c r="C133" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D133" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="E133">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F133" t="b">
         <v>0</v>
@@ -5298,10 +5319,10 @@
         <v>104</v>
       </c>
       <c r="C134" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D134" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="E134">
         <v>5</v>
@@ -5324,13 +5345,13 @@
         <v>104</v>
       </c>
       <c r="C135" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D135" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="E135">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F135" t="b">
         <v>0</v>
@@ -5350,13 +5371,13 @@
         <v>104</v>
       </c>
       <c r="C136" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D136" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E136">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F136" t="b">
         <v>0</v>
@@ -5376,7 +5397,7 @@
         <v>104</v>
       </c>
       <c r="C137" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D137" t="s">
         <v>7</v>
@@ -5402,13 +5423,13 @@
         <v>104</v>
       </c>
       <c r="C138" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D138" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="E138">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="F138" t="b">
         <v>0</v>
@@ -5428,13 +5449,13 @@
         <v>104</v>
       </c>
       <c r="C139" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D139" t="s">
-        <v>113</v>
+        <v>7</v>
       </c>
       <c r="E139">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F139" t="b">
         <v>0</v>
@@ -5454,13 +5475,13 @@
         <v>104</v>
       </c>
       <c r="C140" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D140" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E140">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F140" t="b">
         <v>0</v>
@@ -5483,10 +5504,10 @@
         <v>111</v>
       </c>
       <c r="D141" t="s">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="E141">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="F141" t="b">
         <v>0</v>
@@ -5506,13 +5527,13 @@
         <v>104</v>
       </c>
       <c r="C142" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D142" t="s">
-        <v>7</v>
+        <v>113</v>
       </c>
       <c r="E142">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F142" t="b">
         <v>0</v>
@@ -5532,13 +5553,13 @@
         <v>104</v>
       </c>
       <c r="C143" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D143" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="E143">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F143" t="b">
         <v>0</v>
@@ -5558,13 +5579,13 @@
         <v>104</v>
       </c>
       <c r="C144" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D144" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="E144">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F144" t="b">
         <v>0</v>
@@ -5584,13 +5605,13 @@
         <v>104</v>
       </c>
       <c r="C145" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D145" t="s">
         <v>7</v>
       </c>
       <c r="E145">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F145" t="b">
         <v>0</v>
@@ -5610,13 +5631,13 @@
         <v>104</v>
       </c>
       <c r="C146" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D146" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E146">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F146" t="b">
         <v>0</v>
@@ -5636,13 +5657,13 @@
         <v>104</v>
       </c>
       <c r="C147" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D147" t="s">
-        <v>117</v>
+        <v>6</v>
       </c>
       <c r="E147">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F147" t="b">
         <v>0</v>
@@ -5662,13 +5683,13 @@
         <v>104</v>
       </c>
       <c r="C148" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D148" t="s">
-        <v>119</v>
+        <v>7</v>
       </c>
       <c r="E148">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F148" t="b">
         <v>0</v>
@@ -5688,13 +5709,13 @@
         <v>104</v>
       </c>
       <c r="C149" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D149" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E149">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F149" t="b">
         <v>0</v>
@@ -5714,13 +5735,13 @@
         <v>104</v>
       </c>
       <c r="C150" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D150" t="s">
-        <v>52</v>
+        <v>117</v>
       </c>
       <c r="E150">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="F150" t="b">
         <v>0</v>
@@ -5740,13 +5761,13 @@
         <v>104</v>
       </c>
       <c r="C151" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D151" t="s">
-        <v>6</v>
+        <v>119</v>
       </c>
       <c r="E151">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F151" t="b">
         <v>0</v>
@@ -5766,13 +5787,13 @@
         <v>104</v>
       </c>
       <c r="C152" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D152" t="s">
-        <v>119</v>
+        <v>7</v>
       </c>
       <c r="E152">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F152" t="b">
         <v>0</v>
@@ -5792,13 +5813,13 @@
         <v>104</v>
       </c>
       <c r="C153" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D153" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="E153">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F153" t="b">
         <v>0</v>
@@ -5821,10 +5842,10 @@
         <v>120</v>
       </c>
       <c r="D154" t="s">
-        <v>121</v>
+        <v>6</v>
       </c>
       <c r="E154">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F154" t="b">
         <v>0</v>
@@ -5844,13 +5865,13 @@
         <v>104</v>
       </c>
       <c r="C155" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D155" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="E155">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="F155" t="b">
         <v>0</v>
@@ -5870,13 +5891,13 @@
         <v>104</v>
       </c>
       <c r="C156" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D156" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E156">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F156" t="b">
         <v>0</v>
@@ -5896,13 +5917,13 @@
         <v>104</v>
       </c>
       <c r="C157" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D157" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="E157">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F157" t="b">
         <v>0</v>
@@ -5922,13 +5943,13 @@
         <v>104</v>
       </c>
       <c r="C158" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D158" t="s">
-        <v>119</v>
+        <v>20</v>
       </c>
       <c r="E158">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="F158" t="b">
         <v>0</v>
@@ -5948,13 +5969,13 @@
         <v>104</v>
       </c>
       <c r="C159" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D159" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E159">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F159" t="b">
         <v>0</v>
@@ -5974,7 +5995,7 @@
         <v>104</v>
       </c>
       <c r="C160" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D160" t="s">
         <v>49</v>
@@ -6000,13 +6021,13 @@
         <v>104</v>
       </c>
       <c r="C161" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D161" t="s">
-        <v>6</v>
+        <v>119</v>
       </c>
       <c r="E161">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F161" t="b">
         <v>0</v>
@@ -6026,16 +6047,16 @@
         <v>104</v>
       </c>
       <c r="C162" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D162" t="s">
-        <v>119</v>
+        <v>7</v>
       </c>
       <c r="E162">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F162" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G162">
         <v>0</v>
@@ -6052,13 +6073,13 @@
         <v>104</v>
       </c>
       <c r="C163" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D163" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="E163">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F163" t="b">
         <v>0</v>
@@ -6081,10 +6102,10 @@
         <v>125</v>
       </c>
       <c r="D164" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E164">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F164" t="b">
         <v>0</v>
@@ -6107,13 +6128,13 @@
         <v>125</v>
       </c>
       <c r="D165" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="E165">
         <v>1</v>
       </c>
       <c r="F165" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G165">
         <v>0</v>
@@ -6130,13 +6151,13 @@
         <v>104</v>
       </c>
       <c r="C166" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D166" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
       <c r="E166">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F166" t="b">
         <v>0</v>
@@ -6156,13 +6177,13 @@
         <v>104</v>
       </c>
       <c r="C167" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D167" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="E167">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F167" t="b">
         <v>0</v>
@@ -6182,13 +6203,13 @@
         <v>104</v>
       </c>
       <c r="C168" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D168" t="s">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="E168">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="F168" t="b">
         <v>0</v>
@@ -6208,13 +6229,13 @@
         <v>104</v>
       </c>
       <c r="C169" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D169" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="E169">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F169" t="b">
         <v>0</v>
@@ -6234,13 +6255,13 @@
         <v>104</v>
       </c>
       <c r="C170" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D170" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="E170">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F170" t="b">
         <v>0</v>
@@ -6260,7 +6281,7 @@
         <v>104</v>
       </c>
       <c r="C171" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D171" t="s">
         <v>112</v>
@@ -6286,7 +6307,7 @@
         <v>104</v>
       </c>
       <c r="C172" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D172" t="s">
         <v>113</v>
@@ -6312,13 +6333,13 @@
         <v>104</v>
       </c>
       <c r="C173" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D173" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="E173">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F173" t="b">
         <v>0</v>
@@ -6341,10 +6362,10 @@
         <v>129</v>
       </c>
       <c r="D174" t="s">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="E174">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="F174" t="b">
         <v>0</v>
@@ -6364,13 +6385,13 @@
         <v>104</v>
       </c>
       <c r="C175" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D175" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E175">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="F175" t="b">
         <v>0</v>
@@ -6390,13 +6411,13 @@
         <v>104</v>
       </c>
       <c r="C176" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D176" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="E176">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="F176" t="b">
         <v>0</v>
@@ -6416,7 +6437,7 @@
         <v>104</v>
       </c>
       <c r="C177" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D177" t="s">
         <v>42</v>
@@ -6442,7 +6463,7 @@
         <v>104</v>
       </c>
       <c r="C178" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D178" t="s">
         <v>112</v>
@@ -6468,7 +6489,7 @@
         <v>104</v>
       </c>
       <c r="C179" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D179" t="s">
         <v>113</v>
@@ -6494,7 +6515,7 @@
         <v>104</v>
       </c>
       <c r="C180" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D180" t="s">
         <v>42</v>
@@ -6520,7 +6541,7 @@
         <v>104</v>
       </c>
       <c r="C181" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D181" t="s">
         <v>112</v>
@@ -6546,7 +6567,7 @@
         <v>104</v>
       </c>
       <c r="C182" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D182" t="s">
         <v>113</v>
@@ -6572,7 +6593,7 @@
         <v>104</v>
       </c>
       <c r="C183" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D183" t="s">
         <v>42</v>
@@ -6598,13 +6619,13 @@
         <v>104</v>
       </c>
       <c r="C184" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D184" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="E184">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="F184" t="b">
         <v>0</v>
@@ -6624,16 +6645,16 @@
         <v>104</v>
       </c>
       <c r="C185" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D185" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E185">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="F185" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G185">
         <v>0</v>
@@ -6650,13 +6671,13 @@
         <v>104</v>
       </c>
       <c r="C186" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D186" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="E186">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F186" t="b">
         <v>0</v>
@@ -6679,10 +6700,10 @@
         <v>133</v>
       </c>
       <c r="D187" t="s">
-        <v>134</v>
+        <v>6</v>
       </c>
       <c r="E187">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F187" t="b">
         <v>0</v>
@@ -6702,16 +6723,16 @@
         <v>104</v>
       </c>
       <c r="C188" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D188" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="E188">
-        <v>75</v>
+        <v>1</v>
       </c>
       <c r="F188" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G188">
         <v>0</v>
@@ -6728,13 +6749,13 @@
         <v>104</v>
       </c>
       <c r="C189" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D189" t="s">
-        <v>113</v>
+        <v>7</v>
       </c>
       <c r="E189">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="F189" t="b">
         <v>0</v>
@@ -6754,13 +6775,13 @@
         <v>104</v>
       </c>
       <c r="C190" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D190" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E190">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F190" t="b">
         <v>0</v>
@@ -6783,10 +6804,10 @@
         <v>135</v>
       </c>
       <c r="D191" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
       <c r="E191">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="F191" t="b">
         <v>0</v>
@@ -6809,10 +6830,10 @@
         <v>135</v>
       </c>
       <c r="D192" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="E192">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F192" t="b">
         <v>0</v>
@@ -6835,10 +6856,10 @@
         <v>135</v>
       </c>
       <c r="D193" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E193">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F193" t="b">
         <v>0</v>
@@ -6861,10 +6882,10 @@
         <v>135</v>
       </c>
       <c r="D194" t="s">
-        <v>138</v>
+        <v>25</v>
       </c>
       <c r="E194">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F194" t="b">
         <v>0</v>
@@ -6887,10 +6908,10 @@
         <v>135</v>
       </c>
       <c r="D195" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
       <c r="E195">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F195" t="b">
         <v>0</v>
@@ -6899,7 +6920,7 @@
         <v>0</v>
       </c>
       <c r="H195">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.3">
@@ -6913,19 +6934,19 @@
         <v>135</v>
       </c>
       <c r="D196" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E196">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F196" t="b">
         <v>0</v>
       </c>
       <c r="G196">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H196">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.3">
@@ -6939,7 +6960,7 @@
         <v>135</v>
       </c>
       <c r="D197" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E197">
         <v>5</v>
@@ -6951,24 +6972,24 @@
         <v>0</v>
       </c>
       <c r="H197">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B198" s="2" t="s">
-        <v>142</v>
+      <c r="B198" t="s">
+        <v>104</v>
       </c>
       <c r="C198" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D198" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E198">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F198" t="b">
         <v>0</v>
@@ -6977,47 +6998,47 @@
         <v>0</v>
       </c>
       <c r="H198">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="B199" s="2" t="s">
-        <v>142</v>
+      <c r="B199" t="s">
+        <v>104</v>
       </c>
       <c r="C199" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D199" t="s">
-        <v>42</v>
+        <v>140</v>
       </c>
       <c r="E199">
+        <v>5</v>
+      </c>
+      <c r="F199" t="b">
+        <v>0</v>
+      </c>
+      <c r="G199">
         <v>10</v>
       </c>
-      <c r="F199" t="b">
-        <v>0</v>
-      </c>
-      <c r="G199">
-        <v>0</v>
-      </c>
       <c r="H199">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B200" s="2" t="s">
-        <v>142</v>
+      <c r="B200" t="s">
+        <v>104</v>
       </c>
       <c r="C200" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D200" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="E200">
         <v>5</v>
@@ -7029,7 +7050,7 @@
         <v>0</v>
       </c>
       <c r="H200">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.3">
@@ -7040,13 +7061,13 @@
         <v>142</v>
       </c>
       <c r="C201" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D201" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E201">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F201" t="b">
         <v>0</v>
@@ -7066,10 +7087,10 @@
         <v>142</v>
       </c>
       <c r="C202" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D202" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="E202">
         <v>10</v>
@@ -7092,13 +7113,13 @@
         <v>142</v>
       </c>
       <c r="C203" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D203" t="s">
-        <v>147</v>
+        <v>70</v>
       </c>
       <c r="E203">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F203" t="b">
         <v>0</v>
@@ -7121,10 +7142,10 @@
         <v>145</v>
       </c>
       <c r="D204" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E204">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F204" t="b">
         <v>0</v>
@@ -7144,7 +7165,7 @@
         <v>142</v>
       </c>
       <c r="C205" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D205" t="s">
         <v>59</v>
@@ -7170,10 +7191,10 @@
         <v>142</v>
       </c>
       <c r="C206" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D206" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
       <c r="E206">
         <v>10</v>
@@ -7196,13 +7217,13 @@
         <v>142</v>
       </c>
       <c r="C207" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D207" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E207">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F207" t="b">
         <v>0</v>
@@ -7222,10 +7243,10 @@
         <v>142</v>
       </c>
       <c r="C208" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D208" t="s">
-        <v>144</v>
+        <v>59</v>
       </c>
       <c r="E208">
         <v>10</v>
@@ -7248,7 +7269,7 @@
         <v>142</v>
       </c>
       <c r="C209" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D209" t="s">
         <v>42</v>
@@ -7274,13 +7295,13 @@
         <v>142</v>
       </c>
       <c r="C210" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D210" t="s">
-        <v>62</v>
+        <v>151</v>
       </c>
       <c r="E210">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F210" t="b">
         <v>0</v>
@@ -7300,13 +7321,13 @@
         <v>142</v>
       </c>
       <c r="C211" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D211" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="E211">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F211" t="b">
         <v>0</v>
@@ -7329,10 +7350,10 @@
         <v>152</v>
       </c>
       <c r="D212" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="E212">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F212" t="b">
         <v>0</v>
@@ -7352,13 +7373,13 @@
         <v>142</v>
       </c>
       <c r="C213" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D213" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="E213">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="F213" t="b">
         <v>0</v>
@@ -7378,13 +7399,13 @@
         <v>142</v>
       </c>
       <c r="C214" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D214" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="E214">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F214" t="b">
         <v>0</v>
@@ -7404,16 +7425,16 @@
         <v>142</v>
       </c>
       <c r="C215" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D215" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="E215">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F215" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G215">
         <v>0</v>
@@ -7433,10 +7454,10 @@
         <v>153</v>
       </c>
       <c r="D216" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E216">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F216" t="b">
         <v>0</v>
@@ -7459,10 +7480,10 @@
         <v>153</v>
       </c>
       <c r="D217" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E217">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F217" t="b">
         <v>0</v>
@@ -7479,19 +7500,19 @@
         <v>401</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C218" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D218" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="E218">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F218" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G218">
         <v>0</v>
@@ -7505,16 +7526,16 @@
         <v>402</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C219" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D219" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E219">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F219" t="b">
         <v>0</v>
@@ -7531,16 +7552,16 @@
         <v>403</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C220" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D220" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="E220">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F220" t="b">
         <v>0</v>
@@ -7560,10 +7581,10 @@
         <v>154</v>
       </c>
       <c r="C221" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D221" t="s">
-        <v>7</v>
+        <v>134</v>
       </c>
       <c r="E221">
         <v>5</v>
@@ -7589,10 +7610,10 @@
         <v>156</v>
       </c>
       <c r="D222" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="E222">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F222" t="b">
         <v>0</v>
@@ -7612,7 +7633,7 @@
         <v>154</v>
       </c>
       <c r="C223" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D223" t="s">
         <v>42</v>
@@ -7638,10 +7659,10 @@
         <v>154</v>
       </c>
       <c r="C224" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D224" t="s">
-        <v>158</v>
+        <v>7</v>
       </c>
       <c r="E224">
         <v>5</v>
@@ -7664,10 +7685,10 @@
         <v>154</v>
       </c>
       <c r="C225" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D225" t="s">
-        <v>7</v>
+        <v>134</v>
       </c>
       <c r="E225">
         <v>5</v>
@@ -7693,10 +7714,10 @@
         <v>157</v>
       </c>
       <c r="D226" t="s">
-        <v>134</v>
+        <v>42</v>
       </c>
       <c r="E226">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F226" t="b">
         <v>0</v>
@@ -7716,13 +7737,13 @@
         <v>154</v>
       </c>
       <c r="C227" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D227" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E227">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F227" t="b">
         <v>0</v>
@@ -7742,13 +7763,13 @@
         <v>154</v>
       </c>
       <c r="C228" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D228" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="E228">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F228" t="b">
         <v>0</v>
@@ -7768,13 +7789,13 @@
         <v>154</v>
       </c>
       <c r="C229" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D229" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="E229">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F229" t="b">
         <v>0</v>
@@ -7794,13 +7815,13 @@
         <v>154</v>
       </c>
       <c r="C230" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D230" t="s">
-        <v>7</v>
+        <v>160</v>
       </c>
       <c r="E230">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="F230" t="b">
         <v>0</v>
@@ -7820,13 +7841,13 @@
         <v>154</v>
       </c>
       <c r="C231" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D231" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="E231">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F231" t="b">
         <v>0</v>
@@ -7846,13 +7867,13 @@
         <v>154</v>
       </c>
       <c r="C232" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D232" t="s">
-        <v>163</v>
+        <v>42</v>
       </c>
       <c r="E232">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F232" t="b">
         <v>0</v>
@@ -7872,7 +7893,7 @@
         <v>154</v>
       </c>
       <c r="C233" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D233" t="s">
         <v>7</v>
@@ -7898,13 +7919,13 @@
         <v>154</v>
       </c>
       <c r="C234" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D234" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="E234">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="F234" t="b">
         <v>0</v>
@@ -7924,13 +7945,13 @@
         <v>154</v>
       </c>
       <c r="C235" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D235" t="s">
-        <v>6</v>
+        <v>163</v>
       </c>
       <c r="E235">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F235" t="b">
         <v>0</v>
@@ -7950,13 +7971,13 @@
         <v>154</v>
       </c>
       <c r="C236" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D236" t="s">
-        <v>134</v>
+        <v>7</v>
       </c>
       <c r="E236">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F236" t="b">
         <v>0</v>
@@ -7976,13 +7997,13 @@
         <v>154</v>
       </c>
       <c r="C237" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D237" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E237">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F237" t="b">
         <v>0</v>
@@ -8002,13 +8023,13 @@
         <v>154</v>
       </c>
       <c r="C238" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D238" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="E238">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F238" t="b">
         <v>0</v>
@@ -8028,7 +8049,7 @@
         <v>154</v>
       </c>
       <c r="C239" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D239" t="s">
         <v>134</v>
@@ -8054,13 +8075,13 @@
         <v>154</v>
       </c>
       <c r="C240" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D240" t="s">
+        <v>6</v>
+      </c>
+      <c r="E240">
         <v>25</v>
-      </c>
-      <c r="E240">
-        <v>15</v>
       </c>
       <c r="F240" t="b">
         <v>0</v>
@@ -8080,13 +8101,13 @@
         <v>154</v>
       </c>
       <c r="C241" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D241" t="s">
         <v>42</v>
       </c>
       <c r="E241">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F241" t="b">
         <v>0</v>
@@ -8106,13 +8127,13 @@
         <v>154</v>
       </c>
       <c r="C242" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D242" t="s">
-        <v>59</v>
+        <v>134</v>
       </c>
       <c r="E242">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F242" t="b">
         <v>0</v>
@@ -8135,10 +8156,10 @@
         <v>166</v>
       </c>
       <c r="D243" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="E243">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F243" t="b">
         <v>0</v>
@@ -8158,13 +8179,13 @@
         <v>154</v>
       </c>
       <c r="C244" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D244" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="E244">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F244" t="b">
         <v>0</v>
@@ -8184,13 +8205,13 @@
         <v>154</v>
       </c>
       <c r="C245" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D245" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="E245">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="F245" t="b">
         <v>0</v>
@@ -8210,13 +8231,13 @@
         <v>154</v>
       </c>
       <c r="C246" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D246" t="s">
-        <v>134</v>
+        <v>7</v>
       </c>
       <c r="E246">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F246" t="b">
         <v>0</v>
@@ -8239,10 +8260,10 @@
         <v>167</v>
       </c>
       <c r="D247" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E247">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F247" t="b">
         <v>0</v>
@@ -8265,13 +8286,13 @@
         <v>167</v>
       </c>
       <c r="D248" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="E248">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F248" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G248">
         <v>0</v>
@@ -8285,16 +8306,16 @@
         <v>432</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C249" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D249" t="s">
-        <v>42</v>
+        <v>134</v>
       </c>
       <c r="E249">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F249" t="b">
         <v>0</v>
@@ -8311,16 +8332,16 @@
         <v>433</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C250" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D250" t="s">
-        <v>170</v>
+        <v>7</v>
       </c>
       <c r="E250">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F250" t="b">
         <v>0</v>
@@ -8337,19 +8358,19 @@
         <v>434</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C251" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D251" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E251">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F251" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G251">
         <v>0</v>
@@ -8366,13 +8387,13 @@
         <v>168</v>
       </c>
       <c r="C252" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D252" t="s">
-        <v>170</v>
+        <v>42</v>
       </c>
       <c r="E252">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F252" t="b">
         <v>0</v>
@@ -8392,10 +8413,10 @@
         <v>168</v>
       </c>
       <c r="C253" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D253" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E253">
         <v>5</v>
@@ -8418,13 +8439,13 @@
         <v>168</v>
       </c>
       <c r="C254" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D254" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="E254">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F254" t="b">
         <v>0</v>
@@ -8444,16 +8465,16 @@
         <v>168</v>
       </c>
       <c r="C255" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D255" t="s">
         <v>170</v>
       </c>
       <c r="E255">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F255" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G255">
         <v>0</v>
@@ -8470,13 +8491,13 @@
         <v>168</v>
       </c>
       <c r="C256" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D256" t="s">
         <v>172</v>
       </c>
       <c r="E256">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F256" t="b">
         <v>0</v>
@@ -8496,13 +8517,13 @@
         <v>168</v>
       </c>
       <c r="C257" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D257" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E257">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F257" t="b">
         <v>0</v>
@@ -8522,16 +8543,16 @@
         <v>168</v>
       </c>
       <c r="C258" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D258" t="s">
-        <v>6</v>
+        <v>170</v>
       </c>
       <c r="E258">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="F258" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G258">
         <v>0</v>
@@ -8548,16 +8569,16 @@
         <v>168</v>
       </c>
       <c r="C259" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D259" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E259">
         <v>1</v>
       </c>
       <c r="F259" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G259">
         <v>0</v>
@@ -8577,10 +8598,10 @@
         <v>174</v>
       </c>
       <c r="D260" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E260">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="F260" t="b">
         <v>0</v>
@@ -8600,13 +8621,13 @@
         <v>168</v>
       </c>
       <c r="C261" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D261" t="s">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="E261">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F261" t="b">
         <v>0</v>
@@ -8626,16 +8647,16 @@
         <v>168</v>
       </c>
       <c r="C262" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D262" t="s">
         <v>170</v>
       </c>
       <c r="E262">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F262" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G262">
         <v>0</v>
@@ -8652,13 +8673,13 @@
         <v>168</v>
       </c>
       <c r="C263" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D263" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E263">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F263" t="b">
         <v>0</v>
@@ -8678,13 +8699,13 @@
         <v>168</v>
       </c>
       <c r="C264" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D264" t="s">
-        <v>170</v>
+        <v>42</v>
       </c>
       <c r="E264">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F264" t="b">
         <v>0</v>
@@ -8704,16 +8725,16 @@
         <v>168</v>
       </c>
       <c r="C265" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D265" t="s">
         <v>170</v>
       </c>
       <c r="E265">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F265" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G265">
         <v>0</v>
@@ -8730,13 +8751,13 @@
         <v>168</v>
       </c>
       <c r="C266" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D266" t="s">
-        <v>178</v>
+        <v>25</v>
       </c>
       <c r="E266">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F266" t="b">
         <v>0</v>
@@ -8752,17 +8773,17 @@
       <c r="A267" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B267" t="s">
-        <v>179</v>
+      <c r="B267" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="C267" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D267" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="E267">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="F267" t="b">
         <v>0</v>
@@ -8778,20 +8799,20 @@
       <c r="A268" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="B268" t="s">
-        <v>179</v>
+      <c r="B268" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="C268" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D268" t="s">
-        <v>42</v>
+        <v>170</v>
       </c>
       <c r="E268">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F268" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G268">
         <v>0</v>
@@ -8804,17 +8825,17 @@
       <c r="A269" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="B269" t="s">
-        <v>179</v>
+      <c r="B269" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="C269" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D269" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="E269">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F269" t="b">
         <v>0</v>
@@ -8837,10 +8858,10 @@
         <v>180</v>
       </c>
       <c r="D270" t="s">
-        <v>28</v>
+        <v>181</v>
       </c>
       <c r="E270">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="F270" t="b">
         <v>0</v>
@@ -8863,10 +8884,10 @@
         <v>180</v>
       </c>
       <c r="D271" t="s">
-        <v>70</v>
+        <v>462</v>
       </c>
       <c r="E271">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F271" t="b">
         <v>0</v>
@@ -8886,7 +8907,7 @@
         <v>179</v>
       </c>
       <c r="C272" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D272" t="s">
         <v>42</v>
@@ -8912,7 +8933,7 @@
         <v>179</v>
       </c>
       <c r="C273" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D273" t="s">
         <v>158</v>
@@ -8938,10 +8959,10 @@
         <v>179</v>
       </c>
       <c r="C274" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D274" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="E274">
         <v>5</v>
@@ -8964,7 +8985,7 @@
         <v>179</v>
       </c>
       <c r="C275" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D275" t="s">
         <v>70</v>
@@ -8979,6 +9000,110 @@
         <v>0</v>
       </c>
       <c r="H275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A276" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B276" t="s">
+        <v>179</v>
+      </c>
+      <c r="C276" t="s">
+        <v>182</v>
+      </c>
+      <c r="D276" t="s">
+        <v>42</v>
+      </c>
+      <c r="E276">
+        <v>10</v>
+      </c>
+      <c r="F276" t="b">
+        <v>0</v>
+      </c>
+      <c r="G276">
+        <v>0</v>
+      </c>
+      <c r="H276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A277" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B277" t="s">
+        <v>179</v>
+      </c>
+      <c r="C277" t="s">
+        <v>182</v>
+      </c>
+      <c r="D277" t="s">
+        <v>158</v>
+      </c>
+      <c r="E277">
+        <v>5</v>
+      </c>
+      <c r="F277" t="b">
+        <v>0</v>
+      </c>
+      <c r="G277">
+        <v>0</v>
+      </c>
+      <c r="H277">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A278" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="B278" t="s">
+        <v>179</v>
+      </c>
+      <c r="C278" t="s">
+        <v>182</v>
+      </c>
+      <c r="D278" t="s">
+        <v>70</v>
+      </c>
+      <c r="E278">
+        <v>5</v>
+      </c>
+      <c r="F278" t="b">
+        <v>0</v>
+      </c>
+      <c r="G278">
+        <v>0</v>
+      </c>
+      <c r="H278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A279" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B279" t="s">
+        <v>179</v>
+      </c>
+      <c r="C279" t="s">
+        <v>183</v>
+      </c>
+      <c r="D279" t="s">
+        <v>70</v>
+      </c>
+      <c r="E279">
+        <v>5</v>
+      </c>
+      <c r="F279" t="b">
+        <v>0</v>
+      </c>
+      <c r="G279">
+        <v>0</v>
+      </c>
+      <c r="H279">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
comments, code clean up and bug fixes
</commit_message>
<xml_diff>
--- a/src/mesbg_options.xlsx
+++ b/src/mesbg_options.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF178789-835C-40C0-A828-0EE78D0A6AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3440B9-48DE-4FBD-B0BF-4B8E65ED6CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2C0E6438-1EB7-4493-91C9-83873EACB085}"/>
   </bookViews>
@@ -1839,8 +1839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{301D72E7-4EC7-4027-A18B-32FBE399A765}">
   <dimension ref="A1:H279"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2032,7 +2032,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -4216,7 +4216,7 @@
         <v>0</v>
       </c>
       <c r="H91">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>